<commit_message>
Push baru buat di up
</commit_message>
<xml_diff>
--- a/SEMESTER 1/METODOLOGI PENELITIAN/DataBase Survey Paper-Machine Learning and Signal Processing-Tobias Mikha S.xlsx
+++ b/SEMESTER 1/METODOLOGI PENELITIAN/DataBase Survey Paper-Machine Learning and Signal Processing-Tobias Mikha S.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\S2-Pascasarjana\SEMESTER 1\METODOLOGI PENELITIAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095C9EB7-B007-42B9-83F5-CEAEDA9B0A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7424BF6A-90CD-4946-9801-1A2C2F63383B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,11 +22,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'ML, DL, Preprocessing'!$A$2:$I$21</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="201">
   <si>
     <t>No.</t>
   </si>
@@ -1054,12 +1055,55 @@
   <si>
     <t>Sinyal EEG yang digunakan sudah preprocessed sehingga hasil yang didapat baik. Pada penelitian ini hanya membandingkan akurasi sinyal EEG untuk klasifikasi emosi. Model deep learningnya tidak terdapat perubahan</t>
   </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/10365633</t>
+  </si>
+  <si>
+    <t>https://ijeecs.iaescore.com/index.php/IJEECS/article/view/36676</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2302.09566</t>
+  </si>
+  <si>
+    <t>https://www.frontiersin.org/journals/neuroscience/articles/10.3389/fnins.2020.622759/full</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/9445187</t>
+  </si>
+  <si>
+    <t>KLASIFIKASI TEKS BERITA BERBAHASA INDONESIA MENGGUNAKAN MACHINE LEARNING DAN DEEP LEARNING: STUDI LITERATUR</t>
+  </si>
+  <si>
+    <t>Alfando, Regiolina Hayami ; JATI (Jurnal Mahasiswa Teknik Informatika) Vol. 7 No. 1, Februari 2023</t>
+  </si>
+  <si>
+    <t>Banyak model machine learning untuk melakukan klasifikasi text. Dalam paper ini, membandingkan akurasi dan keandalan model yang sering digunakan untuk melakukan pemodelan text</t>
+  </si>
+  <si>
+    <t>Pada paper ini menjelaskan bahwa SVM memiliki keandalan untuk memproses data text. Dan dijelaskan juga untuk kelebihan dan kekurangan model yang lain</t>
+  </si>
+  <si>
+    <t>Punctual Removal, Case Folding, Tokenization,
+Stopword Removal, Stemming, Support Vector Machine (SVM), K-Nearest Neighbor (KNN), Naïve Bayes Classifier, Long Short-Term Memory, Convolutional Long Short-Term Memory, Multi Layer Perceptron</t>
+  </si>
+  <si>
+    <t>Penggunaan preprocessing data sangat berpengaruh terhadap tingkat akurasi dari model yang dibuat. Keseimbangan data untuk train, test, dan validation serta pemilihan model menjadi parameter untuk dapat meningkatkan akurasi</t>
+  </si>
+  <si>
+    <t>Pemilihan dataset yang digunakan adalah text dengan bahasa indonesia, apabila menggunakan text dengan bahasa inggris, belum tentu model yang dibuat sesuai</t>
+  </si>
+  <si>
+    <t>https://ejournal.itn.ac.id/index.php/jati/article/download/6486/3740</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1116,6 +1160,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1137,7 +1190,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1318,15 +1371,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1365,28 +1409,63 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
@@ -1408,17 +1487,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
@@ -1459,13 +1532,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1487,22 +1557,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1512,17 +1576,46 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1828,8 +1921,8 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1842,6 +1935,7 @@
     <col min="6" max="6" width="36.85546875" customWidth="1"/>
     <col min="7" max="7" width="50.7109375" customWidth="1"/>
     <col min="8" max="8" width="44.28515625" customWidth="1"/>
+    <col min="9" max="9" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1867,606 +1961,693 @@
       <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="14"/>
+      <c r="I2" s="51" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="44" t="s">
         <v>157</v>
       </c>
+      <c r="I3" s="57" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="44" t="s">
         <v>164</v>
       </c>
+      <c r="I4" s="57" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="44" t="s">
         <v>172</v>
       </c>
+      <c r="I5" s="57" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="44" t="s">
         <v>179</v>
       </c>
+      <c r="I6" s="57" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="44" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="I7" s="57" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="8"/>
+      <c r="B8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C8" t="s">
+        <v>194</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="H8" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="I8" s="57" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="52"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="8"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="52"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="8"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="52"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="8"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="52"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="52"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="8"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="52"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="8"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="52"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="8"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="8"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="8"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="8"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="8"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="8"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="8"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="8"/>
-    </row>
-    <row r="25" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="38"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="8"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="8"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="8"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="8"/>
-    </row>
-    <row r="30" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="40"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="42"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="32"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="39"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="32"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="32"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="32"/>
-    </row>
-    <row r="35" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="40"/>
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="42"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="32"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="32"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="30"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="32"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="32"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="30"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="32"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="32"/>
-    </row>
-    <row r="42" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="43"/>
-      <c r="B42" s="44"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44"/>
-      <c r="F42" s="44"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="45"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
-      <c r="B43" s="31"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="32"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
-      <c r="B44" s="31"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="32"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="30"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="32"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="30"/>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="32"/>
-    </row>
-    <row r="47" spans="1:8" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="47"/>
-      <c r="B47" s="48"/>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="48"/>
-      <c r="G47" s="48"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="52"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="52"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="52"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="52"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="52"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="52"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="52"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="52"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="52"/>
+    </row>
+    <row r="25" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="31"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="53"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="52"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="52"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="52"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="52"/>
+    </row>
+    <row r="30" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="36"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="53"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="27"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="52"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="27"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="52"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="27"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="52"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="27"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="52"/>
+    </row>
+    <row r="35" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="36"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="53"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="27"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="52"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="27"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="47"/>
+      <c r="I37" s="52"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="27"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="52"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="27"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="47"/>
+      <c r="I39" s="52"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="27"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="52"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="27"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="47"/>
+      <c r="I41" s="52"/>
+    </row>
+    <row r="42" spans="1:9" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="38"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="48"/>
+      <c r="I42" s="54"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="27"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="47"/>
+      <c r="I43" s="52"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="27"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="47"/>
+      <c r="I44" s="52"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="27"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="47"/>
+      <c r="I45" s="52"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="27"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="28"/>
+      <c r="H46" s="47"/>
+      <c r="I46" s="52"/>
+    </row>
+    <row r="47" spans="1:9" s="40" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="41"/>
+      <c r="B47" s="42"/>
+      <c r="C47" s="42"/>
+      <c r="D47" s="42"/>
+      <c r="E47" s="42"/>
+      <c r="F47" s="42"/>
+      <c r="G47" s="42"/>
       <c r="H47" s="49"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
-      <c r="B48" s="31"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
-      <c r="H48" s="32"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="30"/>
-      <c r="B49" s="31"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="31"/>
-      <c r="H49" s="32"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="30"/>
-      <c r="B50" s="31"/>
-      <c r="C50" s="31"/>
-      <c r="D50" s="31"/>
-      <c r="E50" s="31"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="31"/>
-      <c r="H50" s="32"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="30"/>
-      <c r="B51" s="31"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="31"/>
-      <c r="E51" s="31"/>
-      <c r="F51" s="31"/>
-      <c r="G51" s="31"/>
-      <c r="H51" s="32"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="30"/>
-      <c r="B52" s="31"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="31"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="31"/>
-      <c r="H52" s="32"/>
-    </row>
-    <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="9"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="11"/>
+      <c r="I47" s="54"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="27"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="28"/>
+      <c r="H48" s="47"/>
+      <c r="I48" s="52"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="27"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="47"/>
+      <c r="I49" s="52"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="27"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="47"/>
+      <c r="I50" s="52"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="27"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="47"/>
+      <c r="I51" s="52"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="27"/>
+      <c r="B52" s="28"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="28"/>
+      <c r="H52" s="47"/>
+      <c r="I52" s="52"/>
+    </row>
+    <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="8"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="50"/>
+      <c r="I53" s="52"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I3" r:id="rId1" xr:uid="{718A4EA3-ED1E-444B-9953-D16D7CC9ED18}"/>
+    <hyperlink ref="I4" r:id="rId2" xr:uid="{6B301194-F2BE-4B67-A169-C73A6D89DFF7}"/>
+    <hyperlink ref="I5" r:id="rId3" xr:uid="{0A4D0BE9-BB41-4861-A26C-8819FB86C1B5}"/>
+    <hyperlink ref="I6" r:id="rId4" xr:uid="{7224B9FB-EA6A-4359-BDD2-3311646FB6E5}"/>
+    <hyperlink ref="I7" r:id="rId5" xr:uid="{58E9D6C1-229F-4FC3-A5BC-983D5347EE45}"/>
+    <hyperlink ref="I8" r:id="rId6" xr:uid="{FEEACB7E-1494-4823-8024-5DB93ACF9549}"/>
+  </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -2490,712 +2671,712 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="18" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="240" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="195" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
+      <c r="A8" s="19">
         <v>5</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="21" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
+      <c r="A9" s="19">
         <v>6</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="21" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
+      <c r="A10" s="19">
         <v>7</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="H10" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="21" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
+      <c r="A11" s="19">
         <v>8</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="I11" s="24" t="s">
+      <c r="I11" s="21" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A12" s="22">
+      <c r="A12" s="19">
         <v>9</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="G12" s="23" t="s">
+      <c r="G12" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="H12" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="I12" s="21" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="285" x14ac:dyDescent="0.25">
-      <c r="A13" s="22">
+      <c r="A13" s="19">
         <v>10</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="H13" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="I13" s="24" t="s">
+      <c r="I13" s="21" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>11</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="7" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="8" t="s">
+      <c r="G15" s="6"/>
+      <c r="H15" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="210" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="7" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="7" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="180" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="A18" s="5">
         <v>15</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="180" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+      <c r="A19" s="5">
         <v>16</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="33" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A20" s="35">
+    <row r="20" spans="1:9" s="29" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A20" s="31">
         <v>17</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="36" t="s">
+      <c r="E20" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="F20" s="36" t="s">
+      <c r="F20" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="G20" s="36" t="s">
+      <c r="G20" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="34" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A21" s="22">
+      <c r="A21" s="19">
         <v>18</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="E21" s="23" t="s">
+      <c r="E21" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="G21" s="23" t="s">
+      <c r="G21" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="H21" s="23" t="s">
+      <c r="H21" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="I21" s="24"/>
+      <c r="I21" s="21"/>
     </row>
     <row r="22" spans="1:9" ht="180" x14ac:dyDescent="0.25">
-      <c r="A22" s="22">
+      <c r="A22" s="19">
         <v>19</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="E22" s="23" t="s">
+      <c r="E22" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="F22" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="G22" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="H22" s="23" t="s">
+      <c r="H22" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="I22" s="24"/>
+      <c r="I22" s="21"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="24"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="21"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="24"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="21"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="24"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="21"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="24"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="21"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="24"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="21"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="24"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="21"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="24"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="21"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="24"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="21"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="24"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="21"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="24"/>
+      <c r="A32" s="19"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="21"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="24"/>
+      <c r="A33" s="19"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="21"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="24"/>
+      <c r="A34" s="19"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="21"/>
     </row>
     <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="25"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="27"/>
+      <c r="A35" s="22"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3219,21 +3400,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E8A0BF21F92E044584EDE6E1E83F6A82" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c4a24c2a1376d75c424785819673c65">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1ec4d2c0-4123-4d69-9322-bcf8e0f39d92" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="860a3391895df2b57217a6d53c42d4d8" ns2:_="">
     <xsd:import namespace="1ec4d2c0-4123-4d69-9322-bcf8e0f39d92"/>
@@ -3401,24 +3567,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DA10D09-B341-432C-AFF5-7441712484F0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94F79D63-C803-4F61-9E3A-F43123368083}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67A0EC7F-DED4-4CA3-8E87-86890327AB5E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3434,4 +3598,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DA10D09-B341-432C-AFF5-7441712484F0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94F79D63-C803-4F61-9E3A-F43123368083}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>